<commit_message>
changes in audio agumentations and added new data to xl
</commit_message>
<xml_diff>
--- a/UCLASS.xlsx
+++ b/UCLASS.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1746" uniqueCount="1729">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1967" uniqueCount="1947">
   <si>
     <t>Name</t>
   </si>
@@ -5201,6 +5201,660 @@
   </si>
   <si>
     <t xml:space="preserve">called </t>
+  </si>
+  <si>
+    <t>I  like  to  play  football  for  fun|  and  because</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I  like  to  play  for  fun|  I  normally  </t>
+  </si>
+  <si>
+    <t>BE  on  the  football  team  and</t>
+  </si>
+  <si>
+    <t xml:space="preserve">one  thing  I  like  to  be  on  the  football  team|  because </t>
+  </si>
+  <si>
+    <t xml:space="preserve">you  have  to  LISTEN  and  hear  what  the  coach  is  </t>
+  </si>
+  <si>
+    <t>going to tell  you  er I  don't  know</t>
+  </si>
+  <si>
+    <t>what  to  say!  Er er</t>
+  </si>
+  <si>
+    <t xml:space="preserve">my  favourite  SPORT is  TO  um </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SWIM  because  when  you  swim|  you  get  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">more  ENERGY  in  you  and  after  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">you  swim  you  have  to  TAKE  a  SHOWER  and  rinse  off </t>
+  </si>
+  <si>
+    <t xml:space="preserve">the that  thing  in  the  water. </t>
+  </si>
+  <si>
+    <t>{Prompted by interviewer}  er  er</t>
+  </si>
+  <si>
+    <t>er I  don't  know  what  to  say  about</t>
+  </si>
+  <si>
+    <t xml:space="preserve">football  team| I  like  any  team! </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> {Prompted by interviewer}  My  best  </t>
+  </si>
+  <si>
+    <t>place  I  ever  been|  was  to  er</t>
+  </si>
+  <si>
+    <t>LEGO</t>
+  </si>
+  <si>
+    <t>LAND.  After  we  WENT  there|</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the  next  holiday  we  went  to </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CHESSINGTON  and  then  the  </t>
+  </si>
+  <si>
+    <t>Easter  holidays  we  went  to  Thorpe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Park  in  the  MORNING  and  we 	 </t>
+  </si>
+  <si>
+    <t>CAME  back  something  to  nine  in  the  afternoon.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">And the rides was </t>
+  </si>
+  <si>
+    <t xml:space="preserve">fun.  My  favourite  ride  was  the  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">scary  ride|  where  you  have  to  go  ON  </t>
+  </si>
+  <si>
+    <t>this  ride  and  you  have  to  go  upside  down.</t>
+  </si>
+  <si>
+    <t>computer gmaes, intervier what is you fac foot ball team</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> {Prompted by interviewer}    I  don't  have a </t>
+  </si>
+  <si>
+    <t>Um a few D DAYS ago</t>
+  </si>
+  <si>
+    <t>MIN M MY nan went to Toys r</t>
+  </si>
+  <si>
+    <t>us and we walked around the aisles</t>
+  </si>
+  <si>
+    <t>T TRYING to B BUY something for</t>
+  </si>
+  <si>
+    <t>my birthday and then as we turned the aisle</t>
+  </si>
+  <si>
+    <t>WHERE WHERE we noticed a section that</t>
+  </si>
+  <si>
+    <t>had a G GAMEBOY sign on it. We</t>
+  </si>
+  <si>
+    <t xml:space="preserve">err wum went to it and then I asked </t>
+  </si>
+  <si>
+    <t xml:space="preserve">could we buy the Pokemon G </t>
+  </si>
+  <si>
+    <t xml:space="preserve">GAMEBOY and err um </t>
+  </si>
+  <si>
+    <t>H SH SHE said but look over here THERE'S</t>
+  </si>
+  <si>
+    <t>THE THERE'S a sign saying B BUY two save</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ten pounds so we bought two </t>
+  </si>
+  <si>
+    <t xml:space="preserve">and we paid to the shop assistant </t>
+  </si>
+  <si>
+    <t>and we walked round the bend and then we got these slips</t>
+  </si>
+  <si>
+    <t xml:space="preserve">of P PAPER and these red </t>
+  </si>
+  <si>
+    <t>disc and this B BLUE disc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">After that we W WALKED out and I </t>
+  </si>
+  <si>
+    <t xml:space="preserve">found a card in this W BOOK in this </t>
+  </si>
+  <si>
+    <t xml:space="preserve">trolley and then we ran back home </t>
+  </si>
+  <si>
+    <t>and then after hour at home</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We WE went T TO see the a </t>
+  </si>
+  <si>
+    <t xml:space="preserve">movie. The pokemon movie. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">And then I I got a free card in it. </t>
+  </si>
+  <si>
+    <t>The movie was great but not W WHAT I E</t>
+  </si>
+  <si>
+    <t>ES EXPECTED.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">um| af </t>
+  </si>
+  <si>
+    <t xml:space="preserve">T TER that we W WENT home and </t>
+  </si>
+  <si>
+    <t xml:space="preserve">watched another film called Godzilla </t>
+  </si>
+  <si>
+    <t xml:space="preserve">and then but my baby S SISTER </t>
+  </si>
+  <si>
+    <t xml:space="preserve">couldn't watch it because it was too  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Um| really| last holiday </t>
+  </si>
+  <si>
+    <t>I went to America to see my auntie and uncle.</t>
+  </si>
+  <si>
+    <t>And um| she has</t>
+  </si>
+  <si>
+    <t>a cat and three dogs| it SSSO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Awiming pool.  And </t>
+  </si>
+  <si>
+    <t>we went to the ice-cream parlour a lot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">and um but it was so hot </t>
+  </si>
+  <si>
+    <t>over there um the ice-cream M{x6} MA MELTED.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">But my F FAVOUROTE part is when we went to this um| </t>
+  </si>
+  <si>
+    <t xml:space="preserve">water park and there was this big wave machine </t>
+  </si>
+  <si>
+    <t>and one wave came every er</t>
+  </si>
+  <si>
+    <t>one second|</t>
+  </si>
+  <si>
+    <t xml:space="preserve">er I mean| I mean every five M M </t>
+  </si>
+  <si>
+    <t xml:space="preserve">MINUTES and it was a big tidal wave and it went over my </t>
+  </si>
+  <si>
+    <t xml:space="preserve">dad's head| so it was really tall. </t>
+  </si>
+  <si>
+    <t>Um| I| there was</t>
+  </si>
+  <si>
+    <t xml:space="preserve">once when I was taking Laddy| a dog| out for </t>
+  </si>
+  <si>
+    <t xml:space="preserve">a walk and we| and then we saw this big </t>
+  </si>
+  <si>
+    <t xml:space="preserve">hornet| well it wasn't a hornet| </t>
+  </si>
+  <si>
+    <t>it was CH TWICE as big as a hornet.  And it</t>
+  </si>
+  <si>
+    <t xml:space="preserve">landed right in F F FRONT of  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">LLLADDY| the dog| and we um| I </t>
+  </si>
+  <si>
+    <t xml:space="preserve">just ran up the hill and LL LADDY just sat there </t>
+  </si>
+  <si>
+    <t xml:space="preserve">puzzled.  Um| </t>
+  </si>
+  <si>
+    <t>when I got to the car park I realised I hadn't had</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L LADDY with me and he was still down there with that </t>
+  </si>
+  <si>
+    <t xml:space="preserve">thing.  So I had to WALK WALK </t>
+  </si>
+  <si>
+    <t xml:space="preserve">bravely down there and get him again. </t>
+  </si>
+  <si>
+    <t>Um| we also SSAwam in the lake.</t>
+  </si>
+  <si>
+    <t>noise</t>
+  </si>
+  <si>
+    <t>and um he used to um S SIT on M MY lap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">W WE got quite attached </t>
+  </si>
+  <si>
+    <t xml:space="preserve">IT'S a L LASSIE breed and um </t>
+  </si>
+  <si>
+    <t xml:space="preserve">L LADDIE this um one dog that she has I </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Um </t>
+  </si>
+  <si>
+    <t>and that why she has L LOTS of animals.</t>
+  </si>
+  <si>
+    <t>a guide dog and N animal worker vet person</t>
+  </si>
+  <si>
+    <t>Iâ€™m N NOT sure if this true or not</t>
+  </si>
+  <si>
+    <t>she's a um</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the barking. and um </t>
+  </si>
+  <si>
+    <t>SHE HA SO she had to cough to sad up</t>
+  </si>
+  <si>
+    <t xml:space="preserve">people it SA SA STARTED to bark so she </t>
+  </si>
+  <si>
+    <t>so when she went up in the elevator with other</t>
+  </si>
+  <si>
+    <t xml:space="preserve">W WASN'T allowed and then she hid it in the bag </t>
+  </si>
+  <si>
+    <t>to T TA TAKE it in a hotel with her that</t>
+  </si>
+  <si>
+    <t>a dog with three legs and she had</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uh WW A ADOPTED a W um </t>
+  </si>
+  <si>
+    <t>dogs and a cat but then she</t>
+  </si>
+  <si>
+    <t xml:space="preserve">um used to have two </t>
+  </si>
+  <si>
+    <t xml:space="preserve">my aunty W W </t>
+  </si>
+  <si>
+    <t>L LOOKING F FORWARD to it.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N NINE months and I'm really </t>
+  </si>
+  <si>
+    <t>and she said wâ€™m going to have it in uh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">that that I had a baby C COUSIN </t>
+  </si>
+  <si>
+    <t xml:space="preserve">when I um| w um knew </t>
+  </si>
+  <si>
+    <t>weeks ago I couldn't I was S SPEECHLESS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">was taken pregnant two </t>
+  </si>
+  <si>
+    <t xml:space="preserve">So when my um W um aunty </t>
+  </si>
+  <si>
+    <t>on my mum's side of the family I have none.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DAD'S er side of the family.But </t>
+  </si>
+  <si>
+    <t>um I have six cousins on my er DA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I like </t>
+  </si>
+  <si>
+    <t>um quite a lot of sports most sports really but my favourite is tennis.</t>
+  </si>
+  <si>
+    <t>I play quite a lot in the week| and all the time on the weekends.</t>
+  </si>
+  <si>
+    <t>At school they don't really do much tennis|</t>
+  </si>
+  <si>
+    <t xml:space="preserve">but (ER) at school they do um wide variety of </t>
+  </si>
+  <si>
+    <t xml:space="preserve">sports| such as football| rugby| athletics| </t>
+  </si>
+  <si>
+    <t xml:space="preserve">an cricket. I'm in all those teams| apart from athletics </t>
+  </si>
+  <si>
+    <t xml:space="preserve">which I don't really like. In rugby I play </t>
+  </si>
+  <si>
+    <t>inside centre| which is</t>
+  </si>
+  <si>
+    <t xml:space="preserve">um really kind of (ER) forward| but erm helps at the back as </t>
+  </si>
+  <si>
+    <t>well| midfield if you're talking football wise. In football</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I'm a defender| and I play for the school team as well. In </t>
+  </si>
+  <si>
+    <t>cricket I'm not really er a bowler| but I can bowl quite well|</t>
+  </si>
+  <si>
+    <t xml:space="preserve">quite accurately| I'm more of a batter| and my </t>
+  </si>
+  <si>
+    <t>favourite bat is the v sixhundred by Slazenger.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hu at school my favourite SSSSUBJECT is </t>
+  </si>
+  <si>
+    <t>science| and I like that because you</t>
+  </si>
+  <si>
+    <t>get to find out a wide variety of things.I I</t>
+  </si>
+  <si>
+    <t>I like maths um quite a lot as well| I don't know why</t>
+  </si>
+  <si>
+    <t>I just like it. And um my worst subject</t>
+  </si>
+  <si>
+    <t>is probably English or Latin. I don't like Latin â€˜cause very</t>
+  </si>
+  <si>
+    <t>hard| and English I'm just not very good at.</t>
+  </si>
+  <si>
+    <t>Um| at home| I like to play on the</t>
+  </si>
+  <si>
+    <t>computer a lot. I have a playstation| and an n64</t>
+  </si>
+  <si>
+    <t>my favouriteâ€™s the playstation| which I have lots of games on.</t>
+  </si>
+  <si>
+    <t>I like playing on the pc| especially on</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the internet. Iâ€™ve my own e-mail addresses| </t>
+  </si>
+  <si>
+    <t>and I'm hoping to get my er new website done|</t>
+  </si>
+  <si>
+    <t>um| later this year.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">On the </t>
+  </si>
+  <si>
+    <t xml:space="preserve">playstation my favourite game is DU DU DU DU DU </t>
+  </si>
+  <si>
+    <t>WWF smackdown which is a wrestling game| which</t>
+  </si>
+  <si>
+    <t>is quite a recent one. Mum {block}W W ONE my favourite games</t>
+  </si>
+  <si>
+    <t>is resident evil three| it is very gory and has lots of blood.</t>
+  </si>
+  <si>
+    <t>On the n64 my favourite game is James Bond</t>
+  </si>
+  <si>
+    <t>G GO GAR GOLDENEYE| which IZ</t>
+  </si>
+  <si>
+    <t>{block}IZ based on the film erm with Pierce Brosnan starring as</t>
+  </si>
+  <si>
+    <t>Um um MA FA FAVOURITE</t>
+  </si>
+  <si>
+    <t>things um is my|</t>
+  </si>
+  <si>
+    <t>my brother HEâ€™S</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HE'S N NICE| </t>
+  </si>
+  <si>
+    <t>I like him A L A LOT</t>
+  </si>
+  <si>
+    <t>but S SOMETIMES he gets on my nerves</t>
+  </si>
+  <si>
+    <t>um sometimes I get on</t>
+  </si>
+  <si>
+    <t>his nerves and I L L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LIKE my dad. He's| </t>
+  </si>
+  <si>
+    <t xml:space="preserve">he's </t>
+  </si>
+  <si>
+    <t>V VERY nice to me and when I had slides in my</t>
+  </si>
+  <si>
+    <t>MA MA MA MOUTH he said just close</t>
+  </si>
+  <si>
+    <t>your mouth and S SWALLOW.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">and it W W WOORKED </t>
+  </si>
+  <si>
+    <t>and I like my friends Bas-</t>
+  </si>
+  <si>
+    <t>-hir| Mike</t>
+  </si>
+  <si>
+    <t>M MANARD| Sharmad|</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Segam Abdil| </t>
+  </si>
+  <si>
+    <t xml:space="preserve">those are the people who normally </t>
+  </si>
+  <si>
+    <t>play with me and Y YOUSEF and Naja</t>
+  </si>
+  <si>
+    <t xml:space="preserve">and N N NOT Michael </t>
+  </si>
+  <si>
+    <t xml:space="preserve">and L </t>
+  </si>
+  <si>
+    <t xml:space="preserve">LUCAS and I R REALLY L L LIKE my friends </t>
+  </si>
+  <si>
+    <t xml:space="preserve">but. Um </t>
+  </si>
+  <si>
+    <t xml:space="preserve">there's this thing I R R </t>
+  </si>
+  <si>
+    <t>REALLY LA LA LIKE.it is my</t>
+  </si>
+  <si>
+    <t xml:space="preserve">penguin K K KEYRING which is really beautiful </t>
+  </si>
+  <si>
+    <t xml:space="preserve">it's like| like lumpy circle </t>
+  </si>
+  <si>
+    <t xml:space="preserve">with some like W W W W W </t>
+  </si>
+  <si>
+    <t>um| I like Dragonball</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Z Z  because it's like a IT </t>
+  </si>
+  <si>
+    <t>ITâ€™S a  M MANGA</t>
+  </si>
+  <si>
+    <t>it was one of the first M MANGA cartoons</t>
+  </si>
+  <si>
+    <t xml:space="preserve">that came out and </t>
+  </si>
+  <si>
+    <t xml:space="preserve">I like it because it has martial arts and stuff </t>
+  </si>
+  <si>
+    <t>and it has um S SOUNDS</t>
+  </si>
+  <si>
+    <t>F FOR attacks like aahhma-</t>
+  </si>
+  <si>
+    <t>or DUS engage. I and I</t>
+  </si>
+  <si>
+    <t>saws anything in half and</t>
+  </si>
+  <si>
+    <t>my favourite episode was</t>
+  </si>
+  <si>
+    <t xml:space="preserve">W W WHEN Goku this sayen </t>
+  </si>
+  <si>
+    <t>and a sayen is somebody who can|</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WHO WHOSE WHO </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAN do all stuff like the keoking attack </t>
+  </si>
+  <si>
+    <t>which is a special move that sayens can do.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">And| and goku  WHO </t>
+  </si>
+  <si>
+    <t>WHO is a sayen| he</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WA and HE HE </t>
+  </si>
+  <si>
+    <t>wasn't a super sayen SE AND AND</t>
+  </si>
+  <si>
+    <t>this is quite strange. His  his eyes turned|</t>
+  </si>
+  <si>
+    <t xml:space="preserve">his eyes turned| what's the colour again? oh yeah| </t>
+  </si>
+  <si>
+    <t>his eyes turned green TH HIS eyelid.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Um his </t>
+  </si>
+  <si>
+    <t>eyebrows  turn Y YELLOW so does his hair</t>
+  </si>
+  <si>
+    <t xml:space="preserve">and his| and his M M </t>
+  </si>
+  <si>
+    <t>MUSSES M MUSCLES get stronger and</t>
+  </si>
+  <si>
+    <t>AND AND he can do M MORE attacks</t>
+  </si>
+  <si>
+    <t>THAN THAN a just a sayen and</t>
+  </si>
+  <si>
+    <t>ya or EXTRUCT</t>
   </si>
 </sst>
 </file>
@@ -6033,8 +6687,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J1038"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F817" sqref="F817"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1017" sqref="B1017"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -13914,1105 +14568,1768 @@
       <c r="A818" t="s">
         <v>847</v>
       </c>
+      <c r="B818" t="s">
+        <v>1729</v>
+      </c>
     </row>
     <row r="819" spans="1:2">
       <c r="A819" t="s">
         <v>848</v>
       </c>
+      <c r="B819" t="s">
+        <v>1730</v>
+      </c>
     </row>
     <row r="820" spans="1:2">
       <c r="A820" t="s">
         <v>849</v>
       </c>
+      <c r="B820" t="s">
+        <v>1731</v>
+      </c>
     </row>
     <row r="821" spans="1:2">
       <c r="A821" t="s">
         <v>850</v>
       </c>
+      <c r="B821" t="s">
+        <v>1732</v>
+      </c>
     </row>
     <row r="822" spans="1:2">
       <c r="A822" t="s">
         <v>851</v>
       </c>
+      <c r="B822" t="s">
+        <v>1733</v>
+      </c>
     </row>
     <row r="823" spans="1:2">
       <c r="A823" t="s">
         <v>852</v>
       </c>
+      <c r="B823" t="s">
+        <v>1734</v>
+      </c>
     </row>
     <row r="824" spans="1:2">
       <c r="A824" t="s">
         <v>853</v>
       </c>
+      <c r="B824" t="s">
+        <v>1735</v>
+      </c>
     </row>
     <row r="825" spans="1:2">
       <c r="A825" t="s">
         <v>854</v>
       </c>
+      <c r="B825" t="s">
+        <v>1736</v>
+      </c>
     </row>
     <row r="826" spans="1:2">
       <c r="A826" t="s">
         <v>855</v>
       </c>
+      <c r="B826" t="s">
+        <v>1737</v>
+      </c>
     </row>
     <row r="827" spans="1:2">
       <c r="A827" t="s">
         <v>856</v>
       </c>
+      <c r="B827" t="s">
+        <v>1738</v>
+      </c>
     </row>
     <row r="828" spans="1:2">
       <c r="A828" t="s">
         <v>857</v>
       </c>
+      <c r="B828" t="s">
+        <v>1739</v>
+      </c>
     </row>
     <row r="829" spans="1:2">
       <c r="A829" t="s">
         <v>858</v>
       </c>
+      <c r="B829" t="s">
+        <v>1740</v>
+      </c>
     </row>
     <row r="830" spans="1:2">
       <c r="A830" t="s">
         <v>859</v>
       </c>
+      <c r="B830" t="s">
+        <v>1741</v>
+      </c>
     </row>
     <row r="831" spans="1:2">
       <c r="A831" t="s">
         <v>860</v>
       </c>
+      <c r="B831" t="s">
+        <v>1742</v>
+      </c>
     </row>
     <row r="832" spans="1:2">
       <c r="A832" t="s">
         <v>861</v>
       </c>
-    </row>
-    <row r="833" spans="1:1">
+      <c r="B832" t="s">
+        <v>1757</v>
+      </c>
+    </row>
+    <row r="833" spans="1:2">
       <c r="A833" t="s">
         <v>862</v>
       </c>
-    </row>
-    <row r="834" spans="1:1">
+      <c r="B833" t="s">
+        <v>1758</v>
+      </c>
+    </row>
+    <row r="834" spans="1:2">
       <c r="A834" t="s">
         <v>863</v>
       </c>
-    </row>
-    <row r="835" spans="1:1">
+      <c r="B834" t="s">
+        <v>1743</v>
+      </c>
+    </row>
+    <row r="835" spans="1:2">
       <c r="A835" t="s">
         <v>864</v>
       </c>
-    </row>
-    <row r="836" spans="1:1">
+      <c r="B835" t="s">
+        <v>1744</v>
+      </c>
+    </row>
+    <row r="836" spans="1:2">
       <c r="A836" t="s">
         <v>865</v>
       </c>
-    </row>
-    <row r="837" spans="1:1">
+      <c r="B836" t="s">
+        <v>1745</v>
+      </c>
+    </row>
+    <row r="837" spans="1:2">
       <c r="A837" t="s">
         <v>866</v>
       </c>
-    </row>
-    <row r="838" spans="1:1">
+      <c r="B837" t="s">
+        <v>1746</v>
+      </c>
+    </row>
+    <row r="838" spans="1:2">
       <c r="A838" t="s">
         <v>867</v>
       </c>
-    </row>
-    <row r="839" spans="1:1">
+      <c r="B838" t="s">
+        <v>1747</v>
+      </c>
+    </row>
+    <row r="839" spans="1:2">
       <c r="A839" t="s">
         <v>868</v>
       </c>
-    </row>
-    <row r="840" spans="1:1">
+      <c r="B839" t="s">
+        <v>1748</v>
+      </c>
+    </row>
+    <row r="840" spans="1:2">
       <c r="A840" t="s">
         <v>869</v>
       </c>
-    </row>
-    <row r="841" spans="1:1">
+      <c r="B840" t="s">
+        <v>1749</v>
+      </c>
+    </row>
+    <row r="841" spans="1:2">
       <c r="A841" t="s">
         <v>870</v>
       </c>
-    </row>
-    <row r="842" spans="1:1">
+      <c r="B841" t="s">
+        <v>1750</v>
+      </c>
+    </row>
+    <row r="842" spans="1:2">
       <c r="A842" t="s">
         <v>871</v>
       </c>
-    </row>
-    <row r="843" spans="1:1">
+      <c r="B842" t="s">
+        <v>1751</v>
+      </c>
+    </row>
+    <row r="843" spans="1:2">
       <c r="A843" t="s">
         <v>872</v>
       </c>
-    </row>
-    <row r="844" spans="1:1">
+      <c r="B843" t="s">
+        <v>1752</v>
+      </c>
+    </row>
+    <row r="844" spans="1:2">
       <c r="A844" t="s">
         <v>873</v>
       </c>
-    </row>
-    <row r="845" spans="1:1">
+      <c r="B844" t="s">
+        <v>1753</v>
+      </c>
+    </row>
+    <row r="845" spans="1:2">
       <c r="A845" t="s">
         <v>874</v>
       </c>
-    </row>
-    <row r="846" spans="1:1">
+      <c r="B845" t="s">
+        <v>1754</v>
+      </c>
+    </row>
+    <row r="846" spans="1:2">
       <c r="A846" t="s">
         <v>875</v>
       </c>
-    </row>
-    <row r="847" spans="1:1">
+      <c r="B846" t="s">
+        <v>1755</v>
+      </c>
+    </row>
+    <row r="847" spans="1:2">
       <c r="A847" t="s">
         <v>876</v>
       </c>
-    </row>
-    <row r="848" spans="1:1">
+      <c r="B847" t="s">
+        <v>1756</v>
+      </c>
+    </row>
+    <row r="848" spans="1:2">
       <c r="A848" t="s">
         <v>877</v>
       </c>
-    </row>
-    <row r="849" spans="1:1">
+      <c r="B848" t="s">
+        <v>1759</v>
+      </c>
+    </row>
+    <row r="849" spans="1:2">
       <c r="A849" t="s">
         <v>878</v>
       </c>
-    </row>
-    <row r="850" spans="1:1">
+      <c r="B849" t="s">
+        <v>1760</v>
+      </c>
+    </row>
+    <row r="850" spans="1:2">
       <c r="A850" t="s">
         <v>879</v>
       </c>
-    </row>
-    <row r="851" spans="1:1">
+      <c r="B850" t="s">
+        <v>1761</v>
+      </c>
+    </row>
+    <row r="851" spans="1:2">
       <c r="A851" t="s">
         <v>880</v>
       </c>
-    </row>
-    <row r="852" spans="1:1">
+      <c r="B851" t="s">
+        <v>1762</v>
+      </c>
+    </row>
+    <row r="852" spans="1:2">
       <c r="A852" t="s">
         <v>881</v>
       </c>
-    </row>
-    <row r="853" spans="1:1">
+      <c r="B852" t="s">
+        <v>1763</v>
+      </c>
+    </row>
+    <row r="853" spans="1:2">
       <c r="A853" t="s">
         <v>882</v>
       </c>
-    </row>
-    <row r="854" spans="1:1">
+      <c r="B853" t="s">
+        <v>1764</v>
+      </c>
+    </row>
+    <row r="854" spans="1:2">
       <c r="A854" t="s">
         <v>883</v>
       </c>
-    </row>
-    <row r="855" spans="1:1">
+      <c r="B854" t="s">
+        <v>1765</v>
+      </c>
+    </row>
+    <row r="855" spans="1:2">
       <c r="A855" t="s">
         <v>884</v>
       </c>
-    </row>
-    <row r="856" spans="1:1">
+      <c r="B855" t="s">
+        <v>1766</v>
+      </c>
+    </row>
+    <row r="856" spans="1:2">
       <c r="A856" t="s">
         <v>885</v>
       </c>
-    </row>
-    <row r="857" spans="1:1">
+      <c r="B856" t="s">
+        <v>1767</v>
+      </c>
+    </row>
+    <row r="857" spans="1:2">
       <c r="A857" t="s">
         <v>886</v>
       </c>
-    </row>
-    <row r="858" spans="1:1">
+      <c r="B857" t="s">
+        <v>1768</v>
+      </c>
+    </row>
+    <row r="858" spans="1:2">
       <c r="A858" t="s">
         <v>887</v>
       </c>
-    </row>
-    <row r="859" spans="1:1">
+      <c r="B858" t="s">
+        <v>1769</v>
+      </c>
+    </row>
+    <row r="859" spans="1:2">
       <c r="A859" t="s">
         <v>888</v>
       </c>
-    </row>
-    <row r="860" spans="1:1">
+      <c r="B859" t="s">
+        <v>1770</v>
+      </c>
+    </row>
+    <row r="860" spans="1:2">
       <c r="A860" t="s">
         <v>889</v>
       </c>
-    </row>
-    <row r="861" spans="1:1">
+      <c r="B860" t="s">
+        <v>1771</v>
+      </c>
+    </row>
+    <row r="861" spans="1:2">
       <c r="A861" t="s">
         <v>890</v>
       </c>
-    </row>
-    <row r="862" spans="1:1">
+      <c r="B861" t="s">
+        <v>1772</v>
+      </c>
+    </row>
+    <row r="862" spans="1:2">
       <c r="A862" t="s">
         <v>891</v>
       </c>
-    </row>
-    <row r="863" spans="1:1">
+      <c r="B862" t="s">
+        <v>1773</v>
+      </c>
+    </row>
+    <row r="863" spans="1:2">
       <c r="A863" t="s">
         <v>892</v>
       </c>
-    </row>
-    <row r="864" spans="1:1">
+      <c r="B863" t="s">
+        <v>1774</v>
+      </c>
+    </row>
+    <row r="864" spans="1:2">
       <c r="A864" t="s">
         <v>893</v>
       </c>
-    </row>
-    <row r="865" spans="1:1">
+      <c r="B864" t="s">
+        <v>1775</v>
+      </c>
+    </row>
+    <row r="865" spans="1:2">
       <c r="A865" t="s">
         <v>894</v>
       </c>
-    </row>
-    <row r="866" spans="1:1">
+      <c r="B865" t="s">
+        <v>1776</v>
+      </c>
+    </row>
+    <row r="866" spans="1:2">
       <c r="A866" t="s">
         <v>895</v>
       </c>
-    </row>
-    <row r="867" spans="1:1">
+      <c r="B866" t="s">
+        <v>1777</v>
+      </c>
+    </row>
+    <row r="867" spans="1:2">
       <c r="A867" t="s">
         <v>896</v>
       </c>
-    </row>
-    <row r="868" spans="1:1">
+      <c r="B867" t="s">
+        <v>1778</v>
+      </c>
+    </row>
+    <row r="868" spans="1:2">
       <c r="A868" t="s">
         <v>897</v>
       </c>
-    </row>
-    <row r="869" spans="1:1">
+      <c r="B868" t="s">
+        <v>1779</v>
+      </c>
+    </row>
+    <row r="869" spans="1:2">
       <c r="A869" t="s">
         <v>898</v>
       </c>
-    </row>
-    <row r="870" spans="1:1">
+      <c r="B869" t="s">
+        <v>1780</v>
+      </c>
+    </row>
+    <row r="870" spans="1:2">
       <c r="A870" t="s">
         <v>899</v>
       </c>
-    </row>
-    <row r="871" spans="1:1">
+      <c r="B870" t="s">
+        <v>1781</v>
+      </c>
+    </row>
+    <row r="871" spans="1:2">
       <c r="A871" t="s">
         <v>900</v>
       </c>
-    </row>
-    <row r="872" spans="1:1">
+      <c r="B871" t="s">
+        <v>1782</v>
+      </c>
+    </row>
+    <row r="872" spans="1:2">
       <c r="A872" t="s">
         <v>901</v>
       </c>
-    </row>
-    <row r="873" spans="1:1">
+      <c r="B872" t="s">
+        <v>1783</v>
+      </c>
+    </row>
+    <row r="873" spans="1:2">
       <c r="A873" t="s">
         <v>902</v>
       </c>
-    </row>
-    <row r="874" spans="1:1">
+      <c r="B873" t="s">
+        <v>1784</v>
+      </c>
+    </row>
+    <row r="874" spans="1:2">
       <c r="A874" t="s">
         <v>903</v>
       </c>
-    </row>
-    <row r="875" spans="1:1">
+      <c r="B874" t="s">
+        <v>1785</v>
+      </c>
+    </row>
+    <row r="875" spans="1:2">
       <c r="A875" t="s">
         <v>904</v>
       </c>
-    </row>
-    <row r="876" spans="1:1">
+      <c r="B875" t="s">
+        <v>1786</v>
+      </c>
+    </row>
+    <row r="876" spans="1:2">
       <c r="A876" t="s">
         <v>905</v>
       </c>
-    </row>
-    <row r="877" spans="1:1">
+      <c r="B876" t="s">
+        <v>1787</v>
+      </c>
+    </row>
+    <row r="877" spans="1:2">
       <c r="A877" t="s">
         <v>906</v>
       </c>
-    </row>
-    <row r="878" spans="1:1">
+      <c r="B877" t="s">
+        <v>1788</v>
+      </c>
+    </row>
+    <row r="878" spans="1:2">
       <c r="A878" t="s">
         <v>907</v>
       </c>
-    </row>
-    <row r="879" spans="1:1">
+      <c r="B878" t="s">
+        <v>1789</v>
+      </c>
+    </row>
+    <row r="879" spans="1:2">
       <c r="A879" t="s">
         <v>908</v>
       </c>
-    </row>
-    <row r="880" spans="1:1">
+      <c r="B879" t="s">
+        <v>1790</v>
+      </c>
+    </row>
+    <row r="880" spans="1:2">
       <c r="A880" t="s">
         <v>909</v>
       </c>
-    </row>
-    <row r="881" spans="1:1">
+      <c r="B880" t="s">
+        <v>1791</v>
+      </c>
+    </row>
+    <row r="881" spans="1:2">
       <c r="A881" t="s">
         <v>910</v>
       </c>
-    </row>
-    <row r="882" spans="1:1">
+      <c r="B881" t="s">
+        <v>1792</v>
+      </c>
+    </row>
+    <row r="882" spans="1:2">
       <c r="A882" t="s">
         <v>911</v>
       </c>
-    </row>
-    <row r="883" spans="1:1">
+      <c r="B882" t="s">
+        <v>1793</v>
+      </c>
+    </row>
+    <row r="883" spans="1:2">
       <c r="A883" t="s">
         <v>912</v>
       </c>
-    </row>
-    <row r="884" spans="1:1">
+      <c r="B883" t="s">
+        <v>1794</v>
+      </c>
+    </row>
+    <row r="884" spans="1:2">
       <c r="A884" t="s">
         <v>913</v>
       </c>
-    </row>
-    <row r="885" spans="1:1">
+      <c r="B884" t="s">
+        <v>1795</v>
+      </c>
+    </row>
+    <row r="885" spans="1:2">
       <c r="A885" t="s">
         <v>914</v>
       </c>
-    </row>
-    <row r="886" spans="1:1">
+      <c r="B885" t="s">
+        <v>1796</v>
+      </c>
+    </row>
+    <row r="886" spans="1:2">
       <c r="A886" t="s">
         <v>915</v>
       </c>
-    </row>
-    <row r="887" spans="1:1">
+      <c r="B886" t="s">
+        <v>1797</v>
+      </c>
+    </row>
+    <row r="887" spans="1:2">
       <c r="A887" t="s">
         <v>916</v>
       </c>
-    </row>
-    <row r="888" spans="1:1">
+      <c r="B887" t="s">
+        <v>1798</v>
+      </c>
+    </row>
+    <row r="888" spans="1:2">
       <c r="A888" t="s">
         <v>917</v>
       </c>
-    </row>
-    <row r="889" spans="1:1">
+      <c r="B888" t="s">
+        <v>1799</v>
+      </c>
+    </row>
+    <row r="889" spans="1:2">
       <c r="A889" t="s">
         <v>918</v>
       </c>
-    </row>
-    <row r="890" spans="1:1">
+      <c r="B889" t="s">
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="890" spans="1:2">
       <c r="A890" t="s">
         <v>919</v>
       </c>
-    </row>
-    <row r="891" spans="1:1">
+      <c r="B890" t="s">
+        <v>1801</v>
+      </c>
+    </row>
+    <row r="891" spans="1:2">
       <c r="A891" t="s">
         <v>920</v>
       </c>
-    </row>
-    <row r="892" spans="1:1">
+      <c r="B891" t="s">
+        <v>1802</v>
+      </c>
+    </row>
+    <row r="892" spans="1:2">
       <c r="A892" t="s">
         <v>921</v>
       </c>
-    </row>
-    <row r="893" spans="1:1">
+      <c r="B892" t="s">
+        <v>1803</v>
+      </c>
+    </row>
+    <row r="893" spans="1:2">
       <c r="A893" t="s">
         <v>922</v>
       </c>
-    </row>
-    <row r="894" spans="1:1">
+      <c r="B893" t="s">
+        <v>1804</v>
+      </c>
+    </row>
+    <row r="894" spans="1:2">
       <c r="A894" t="s">
         <v>923</v>
       </c>
-    </row>
-    <row r="895" spans="1:1">
+      <c r="B894" t="s">
+        <v>1805</v>
+      </c>
+    </row>
+    <row r="895" spans="1:2">
       <c r="A895" t="s">
         <v>924</v>
       </c>
-    </row>
-    <row r="896" spans="1:1">
+      <c r="B895" t="s">
+        <v>1806</v>
+      </c>
+    </row>
+    <row r="896" spans="1:2">
       <c r="A896" t="s">
         <v>925</v>
       </c>
-    </row>
-    <row r="897" spans="1:1">
+      <c r="B896" t="s">
+        <v>1807</v>
+      </c>
+    </row>
+    <row r="897" spans="1:2">
       <c r="A897" t="s">
         <v>926</v>
       </c>
-    </row>
-    <row r="898" spans="1:1">
+      <c r="B897" t="s">
+        <v>1808</v>
+      </c>
+    </row>
+    <row r="898" spans="1:2">
       <c r="A898" t="s">
         <v>927</v>
       </c>
-    </row>
-    <row r="899" spans="1:1">
+      <c r="B898" t="s">
+        <v>1809</v>
+      </c>
+    </row>
+    <row r="899" spans="1:2">
       <c r="A899" t="s">
         <v>928</v>
       </c>
-    </row>
-    <row r="900" spans="1:1">
+      <c r="B899" t="s">
+        <v>1810</v>
+      </c>
+    </row>
+    <row r="900" spans="1:2">
       <c r="A900" t="s">
         <v>929</v>
       </c>
-    </row>
-    <row r="901" spans="1:1">
+      <c r="B900" t="s">
+        <v>1811</v>
+      </c>
+    </row>
+    <row r="901" spans="1:2">
       <c r="A901" t="s">
         <v>930</v>
       </c>
-    </row>
-    <row r="902" spans="1:1">
+      <c r="B901" t="s">
+        <v>1812</v>
+      </c>
+    </row>
+    <row r="902" spans="1:2">
       <c r="A902" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="903" spans="1:1">
+      <c r="B902" t="s">
+        <v>1813</v>
+      </c>
+    </row>
+    <row r="903" spans="1:2">
       <c r="A903" t="s">
         <v>932</v>
       </c>
-    </row>
-    <row r="904" spans="1:1">
+      <c r="B903" t="s">
+        <v>1814</v>
+      </c>
+    </row>
+    <row r="904" spans="1:2">
       <c r="A904" t="s">
         <v>933</v>
       </c>
-    </row>
-    <row r="905" spans="1:1">
+      <c r="B904" t="s">
+        <v>1815</v>
+      </c>
+    </row>
+    <row r="905" spans="1:2">
       <c r="A905" t="s">
         <v>934</v>
       </c>
-    </row>
-    <row r="906" spans="1:1">
+      <c r="B905" t="s">
+        <v>1816</v>
+      </c>
+    </row>
+    <row r="906" spans="1:2">
       <c r="A906" t="s">
         <v>935</v>
       </c>
-    </row>
-    <row r="907" spans="1:1">
+      <c r="B906" t="s">
+        <v>1817</v>
+      </c>
+    </row>
+    <row r="907" spans="1:2">
       <c r="A907" t="s">
         <v>936</v>
       </c>
-    </row>
-    <row r="908" spans="1:1">
+      <c r="B907" t="s">
+        <v>1818</v>
+      </c>
+    </row>
+    <row r="908" spans="1:2">
       <c r="A908" t="s">
         <v>937</v>
       </c>
-    </row>
-    <row r="909" spans="1:1">
+      <c r="B908" t="s">
+        <v>1819</v>
+      </c>
+    </row>
+    <row r="909" spans="1:2">
       <c r="A909" t="s">
         <v>938</v>
       </c>
-    </row>
-    <row r="910" spans="1:1">
+      <c r="B909" t="s">
+        <v>1850</v>
+      </c>
+    </row>
+    <row r="910" spans="1:2">
       <c r="A910" t="s">
         <v>939</v>
       </c>
-    </row>
-    <row r="911" spans="1:1">
+      <c r="B910" t="s">
+        <v>1849</v>
+      </c>
+    </row>
+    <row r="911" spans="1:2">
       <c r="A911" t="s">
         <v>940</v>
       </c>
-    </row>
-    <row r="912" spans="1:1">
+      <c r="B911" t="s">
+        <v>1848</v>
+      </c>
+    </row>
+    <row r="912" spans="1:2">
       <c r="A912" t="s">
         <v>941</v>
       </c>
-    </row>
-    <row r="913" spans="1:1">
+      <c r="B912" t="s">
+        <v>1847</v>
+      </c>
+    </row>
+    <row r="913" spans="1:2">
       <c r="A913" t="s">
         <v>942</v>
       </c>
-    </row>
-    <row r="914" spans="1:1">
+      <c r="B913" t="s">
+        <v>1846</v>
+      </c>
+    </row>
+    <row r="914" spans="1:2">
       <c r="A914" t="s">
         <v>943</v>
       </c>
-    </row>
-    <row r="915" spans="1:1">
+      <c r="B914" t="s">
+        <v>1845</v>
+      </c>
+    </row>
+    <row r="915" spans="1:2">
       <c r="A915" t="s">
         <v>944</v>
       </c>
-    </row>
-    <row r="916" spans="1:1">
+      <c r="B915" t="s">
+        <v>1844</v>
+      </c>
+    </row>
+    <row r="916" spans="1:2">
       <c r="A916" t="s">
         <v>945</v>
       </c>
-    </row>
-    <row r="917" spans="1:1">
+      <c r="B916" t="s">
+        <v>1843</v>
+      </c>
+    </row>
+    <row r="917" spans="1:2">
       <c r="A917" t="s">
         <v>946</v>
       </c>
-    </row>
-    <row r="918" spans="1:1">
+      <c r="B917" t="s">
+        <v>1842</v>
+      </c>
+    </row>
+    <row r="918" spans="1:2">
       <c r="A918" t="s">
         <v>947</v>
       </c>
-    </row>
-    <row r="919" spans="1:1">
+      <c r="B918" t="s">
+        <v>1841</v>
+      </c>
+    </row>
+    <row r="919" spans="1:2">
       <c r="A919" t="s">
         <v>948</v>
       </c>
-    </row>
-    <row r="920" spans="1:1">
+      <c r="B919" t="s">
+        <v>1840</v>
+      </c>
+    </row>
+    <row r="920" spans="1:2">
       <c r="A920" t="s">
         <v>949</v>
       </c>
-    </row>
-    <row r="921" spans="1:1">
+      <c r="B920" t="s">
+        <v>1824</v>
+      </c>
+    </row>
+    <row r="921" spans="1:2">
       <c r="A921" t="s">
         <v>950</v>
       </c>
-    </row>
-    <row r="922" spans="1:1">
+      <c r="B921" t="s">
+        <v>1839</v>
+      </c>
+    </row>
+    <row r="922" spans="1:2">
       <c r="A922" t="s">
         <v>951</v>
       </c>
-    </row>
-    <row r="923" spans="1:1">
+      <c r="B922" t="s">
+        <v>1838</v>
+      </c>
+    </row>
+    <row r="923" spans="1:2">
       <c r="A923" t="s">
         <v>952</v>
       </c>
-    </row>
-    <row r="924" spans="1:1">
+      <c r="B923" t="s">
+        <v>1837</v>
+      </c>
+    </row>
+    <row r="924" spans="1:2">
       <c r="A924" t="s">
         <v>953</v>
       </c>
-    </row>
-    <row r="925" spans="1:1">
+      <c r="B924" t="s">
+        <v>1836</v>
+      </c>
+    </row>
+    <row r="925" spans="1:2">
       <c r="A925" t="s">
         <v>954</v>
       </c>
-    </row>
-    <row r="926" spans="1:1">
+      <c r="B925" t="s">
+        <v>1835</v>
+      </c>
+    </row>
+    <row r="926" spans="1:2">
       <c r="A926" t="s">
         <v>955</v>
       </c>
-    </row>
-    <row r="927" spans="1:1">
+      <c r="B926" t="s">
+        <v>1834</v>
+      </c>
+    </row>
+    <row r="927" spans="1:2">
       <c r="A927" t="s">
         <v>956</v>
       </c>
-    </row>
-    <row r="928" spans="1:1">
+      <c r="B927" t="s">
+        <v>1833</v>
+      </c>
+    </row>
+    <row r="928" spans="1:2">
       <c r="A928" t="s">
         <v>957</v>
       </c>
-    </row>
-    <row r="929" spans="1:1">
+      <c r="B928" t="s">
+        <v>1832</v>
+      </c>
+    </row>
+    <row r="929" spans="1:2">
       <c r="A929" t="s">
         <v>958</v>
       </c>
-    </row>
-    <row r="930" spans="1:1">
+      <c r="B929" t="s">
+        <v>1831</v>
+      </c>
+    </row>
+    <row r="930" spans="1:2">
       <c r="A930" t="s">
         <v>959</v>
       </c>
-    </row>
-    <row r="931" spans="1:1">
+      <c r="B930" t="s">
+        <v>1830</v>
+      </c>
+    </row>
+    <row r="931" spans="1:2">
       <c r="A931" t="s">
         <v>960</v>
       </c>
-    </row>
-    <row r="932" spans="1:1">
+      <c r="B931" t="s">
+        <v>1829</v>
+      </c>
+    </row>
+    <row r="932" spans="1:2">
       <c r="A932" t="s">
         <v>961</v>
       </c>
-    </row>
-    <row r="933" spans="1:1">
+      <c r="B932" t="s">
+        <v>1828</v>
+      </c>
+    </row>
+    <row r="933" spans="1:2">
       <c r="A933" t="s">
         <v>962</v>
       </c>
-    </row>
-    <row r="934" spans="1:1">
+      <c r="B933" t="s">
+        <v>1827</v>
+      </c>
+    </row>
+    <row r="934" spans="1:2">
       <c r="A934" t="s">
         <v>963</v>
       </c>
-    </row>
-    <row r="935" spans="1:1">
+      <c r="B934" t="s">
+        <v>1826</v>
+      </c>
+    </row>
+    <row r="935" spans="1:2">
       <c r="A935" t="s">
         <v>964</v>
       </c>
-    </row>
-    <row r="936" spans="1:1">
+      <c r="B935" t="s">
+        <v>1825</v>
+      </c>
+    </row>
+    <row r="936" spans="1:2">
       <c r="A936" t="s">
         <v>965</v>
       </c>
-    </row>
-    <row r="937" spans="1:1">
+      <c r="B936" t="s">
+        <v>1824</v>
+      </c>
+    </row>
+    <row r="937" spans="1:2">
       <c r="A937" t="s">
         <v>966</v>
       </c>
-    </row>
-    <row r="938" spans="1:1">
+      <c r="B937" t="s">
+        <v>1823</v>
+      </c>
+    </row>
+    <row r="938" spans="1:2">
       <c r="A938" t="s">
         <v>967</v>
       </c>
-    </row>
-    <row r="939" spans="1:1">
+      <c r="B938" t="s">
+        <v>1822</v>
+      </c>
+    </row>
+    <row r="939" spans="1:2">
       <c r="A939" t="s">
         <v>968</v>
       </c>
-    </row>
-    <row r="940" spans="1:1">
+      <c r="B939" t="s">
+        <v>1821</v>
+      </c>
+    </row>
+    <row r="940" spans="1:2">
       <c r="A940" t="s">
         <v>969</v>
       </c>
-    </row>
-    <row r="941" spans="1:1">
+      <c r="B940" t="s">
+        <v>1820</v>
+      </c>
+    </row>
+    <row r="941" spans="1:2">
       <c r="A941" t="s">
         <v>970</v>
       </c>
-    </row>
-    <row r="942" spans="1:1">
+      <c r="B941" t="s">
+        <v>1851</v>
+      </c>
+    </row>
+    <row r="942" spans="1:2">
       <c r="A942" t="s">
         <v>971</v>
       </c>
-    </row>
-    <row r="943" spans="1:1">
+      <c r="B942" t="s">
+        <v>1852</v>
+      </c>
+    </row>
+    <row r="943" spans="1:2">
       <c r="A943" t="s">
         <v>972</v>
       </c>
-    </row>
-    <row r="944" spans="1:1">
+      <c r="B943" t="s">
+        <v>1853</v>
+      </c>
+    </row>
+    <row r="944" spans="1:2">
       <c r="A944" t="s">
         <v>973</v>
       </c>
-    </row>
-    <row r="945" spans="1:1">
+      <c r="B944" t="s">
+        <v>1854</v>
+      </c>
+    </row>
+    <row r="945" spans="1:2">
       <c r="A945" t="s">
         <v>974</v>
       </c>
-    </row>
-    <row r="946" spans="1:1">
+      <c r="B945" t="s">
+        <v>1855</v>
+      </c>
+    </row>
+    <row r="946" spans="1:2">
       <c r="A946" t="s">
         <v>975</v>
       </c>
-    </row>
-    <row r="947" spans="1:1">
+      <c r="B946" t="s">
+        <v>1856</v>
+      </c>
+    </row>
+    <row r="947" spans="1:2">
       <c r="A947" t="s">
         <v>976</v>
       </c>
-    </row>
-    <row r="948" spans="1:1">
+      <c r="B947" t="s">
+        <v>1857</v>
+      </c>
+    </row>
+    <row r="948" spans="1:2">
       <c r="A948" t="s">
         <v>977</v>
       </c>
-    </row>
-    <row r="949" spans="1:1">
+      <c r="B948" t="s">
+        <v>1858</v>
+      </c>
+    </row>
+    <row r="949" spans="1:2">
       <c r="A949" t="s">
         <v>978</v>
       </c>
-    </row>
-    <row r="950" spans="1:1">
+      <c r="B949" t="s">
+        <v>1859</v>
+      </c>
+    </row>
+    <row r="950" spans="1:2">
       <c r="A950" t="s">
         <v>979</v>
       </c>
-    </row>
-    <row r="951" spans="1:1">
+      <c r="B950" t="s">
+        <v>1860</v>
+      </c>
+    </row>
+    <row r="951" spans="1:2">
       <c r="A951" t="s">
         <v>980</v>
       </c>
-    </row>
-    <row r="952" spans="1:1">
+      <c r="B951" t="s">
+        <v>1861</v>
+      </c>
+    </row>
+    <row r="952" spans="1:2">
       <c r="A952" t="s">
         <v>981</v>
       </c>
-    </row>
-    <row r="953" spans="1:1">
+      <c r="B952" t="s">
+        <v>1862</v>
+      </c>
+    </row>
+    <row r="953" spans="1:2">
       <c r="A953" t="s">
         <v>982</v>
       </c>
-    </row>
-    <row r="954" spans="1:1">
+      <c r="B953" t="s">
+        <v>1863</v>
+      </c>
+    </row>
+    <row r="954" spans="1:2">
       <c r="A954" t="s">
         <v>983</v>
       </c>
-    </row>
-    <row r="955" spans="1:1">
+      <c r="B954" t="s">
+        <v>1864</v>
+      </c>
+    </row>
+    <row r="955" spans="1:2">
       <c r="A955" t="s">
         <v>984</v>
       </c>
-    </row>
-    <row r="956" spans="1:1">
+      <c r="B955" t="s">
+        <v>1865</v>
+      </c>
+    </row>
+    <row r="956" spans="1:2">
       <c r="A956" t="s">
         <v>985</v>
       </c>
-    </row>
-    <row r="957" spans="1:1">
+      <c r="B956" t="s">
+        <v>1866</v>
+      </c>
+    </row>
+    <row r="957" spans="1:2">
       <c r="A957" t="s">
         <v>986</v>
       </c>
-    </row>
-    <row r="958" spans="1:1">
+      <c r="B957" t="s">
+        <v>1867</v>
+      </c>
+    </row>
+    <row r="958" spans="1:2">
       <c r="A958" t="s">
         <v>987</v>
       </c>
-    </row>
-    <row r="959" spans="1:1">
+      <c r="B958" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="959" spans="1:2">
       <c r="A959" t="s">
         <v>988</v>
       </c>
-    </row>
-    <row r="960" spans="1:1">
+      <c r="B959" t="s">
+        <v>1869</v>
+      </c>
+    </row>
+    <row r="960" spans="1:2">
       <c r="A960" t="s">
         <v>989</v>
       </c>
-    </row>
-    <row r="961" spans="1:1">
+      <c r="B960" t="s">
+        <v>1870</v>
+      </c>
+    </row>
+    <row r="961" spans="1:2">
       <c r="A961" t="s">
         <v>990</v>
       </c>
-    </row>
-    <row r="962" spans="1:1">
+      <c r="B961" t="s">
+        <v>1871</v>
+      </c>
+    </row>
+    <row r="962" spans="1:2">
       <c r="A962" t="s">
         <v>991</v>
       </c>
-    </row>
-    <row r="963" spans="1:1">
+      <c r="B962" t="s">
+        <v>1872</v>
+      </c>
+    </row>
+    <row r="963" spans="1:2">
       <c r="A963" t="s">
         <v>992</v>
       </c>
-    </row>
-    <row r="964" spans="1:1">
+      <c r="B963" t="s">
+        <v>1873</v>
+      </c>
+    </row>
+    <row r="964" spans="1:2">
       <c r="A964" t="s">
         <v>993</v>
       </c>
-    </row>
-    <row r="965" spans="1:1">
+      <c r="B964" t="s">
+        <v>1874</v>
+      </c>
+    </row>
+    <row r="965" spans="1:2">
       <c r="A965" t="s">
         <v>994</v>
       </c>
-    </row>
-    <row r="966" spans="1:1">
+      <c r="B965" t="s">
+        <v>1875</v>
+      </c>
+    </row>
+    <row r="966" spans="1:2">
       <c r="A966" t="s">
         <v>995</v>
       </c>
-    </row>
-    <row r="967" spans="1:1">
+      <c r="B966" t="s">
+        <v>1876</v>
+      </c>
+    </row>
+    <row r="967" spans="1:2">
       <c r="A967" t="s">
         <v>996</v>
       </c>
-    </row>
-    <row r="968" spans="1:1">
+      <c r="B967" t="s">
+        <v>1877</v>
+      </c>
+    </row>
+    <row r="968" spans="1:2">
       <c r="A968" t="s">
         <v>997</v>
       </c>
-    </row>
-    <row r="969" spans="1:1">
+      <c r="B968" t="s">
+        <v>1878</v>
+      </c>
+    </row>
+    <row r="969" spans="1:2">
       <c r="A969" t="s">
         <v>998</v>
       </c>
-    </row>
-    <row r="970" spans="1:1">
+      <c r="B969" t="s">
+        <v>1879</v>
+      </c>
+    </row>
+    <row r="970" spans="1:2">
       <c r="A970" t="s">
         <v>999</v>
       </c>
-    </row>
-    <row r="971" spans="1:1">
+      <c r="B970" t="s">
+        <v>1819</v>
+      </c>
+    </row>
+    <row r="971" spans="1:2">
       <c r="A971" t="s">
         <v>1000</v>
       </c>
-    </row>
-    <row r="972" spans="1:1">
+      <c r="B971" t="s">
+        <v>1880</v>
+      </c>
+    </row>
+    <row r="972" spans="1:2">
       <c r="A972" t="s">
         <v>1001</v>
       </c>
-    </row>
-    <row r="973" spans="1:1">
+      <c r="B972" t="s">
+        <v>1881</v>
+      </c>
+    </row>
+    <row r="973" spans="1:2">
       <c r="A973" t="s">
         <v>1002</v>
       </c>
-    </row>
-    <row r="974" spans="1:1">
+      <c r="B973" t="s">
+        <v>1882</v>
+      </c>
+    </row>
+    <row r="974" spans="1:2">
       <c r="A974" t="s">
         <v>1003</v>
       </c>
-    </row>
-    <row r="975" spans="1:1">
+      <c r="B974" t="s">
+        <v>1883</v>
+      </c>
+    </row>
+    <row r="975" spans="1:2">
       <c r="A975" t="s">
         <v>1004</v>
       </c>
-    </row>
-    <row r="976" spans="1:1">
+      <c r="B975" t="s">
+        <v>1884</v>
+      </c>
+    </row>
+    <row r="976" spans="1:2">
       <c r="A976" t="s">
         <v>1005</v>
       </c>
-    </row>
-    <row r="977" spans="1:1">
+      <c r="B976" t="s">
+        <v>1885</v>
+      </c>
+    </row>
+    <row r="977" spans="1:2">
       <c r="A977" t="s">
         <v>1006</v>
       </c>
-    </row>
-    <row r="978" spans="1:1">
+      <c r="B977" t="s">
+        <v>1886</v>
+      </c>
+    </row>
+    <row r="978" spans="1:2">
       <c r="A978" t="s">
         <v>1007</v>
       </c>
-    </row>
-    <row r="979" spans="1:1">
+      <c r="B978" t="s">
+        <v>1887</v>
+      </c>
+    </row>
+    <row r="979" spans="1:2">
       <c r="A979" t="s">
         <v>1008</v>
       </c>
-    </row>
-    <row r="980" spans="1:1">
+      <c r="B979" t="s">
+        <v>1888</v>
+      </c>
+    </row>
+    <row r="980" spans="1:2">
       <c r="A980" t="s">
         <v>1009</v>
       </c>
-    </row>
-    <row r="981" spans="1:1">
+      <c r="B980" t="s">
+        <v>1889</v>
+      </c>
+    </row>
+    <row r="981" spans="1:2">
       <c r="A981" t="s">
         <v>1010</v>
       </c>
-    </row>
-    <row r="982" spans="1:1">
+      <c r="B981" t="s">
+        <v>1890</v>
+      </c>
+    </row>
+    <row r="982" spans="1:2">
       <c r="A982" t="s">
         <v>1011</v>
       </c>
-    </row>
-    <row r="983" spans="1:1">
+      <c r="B982" t="s">
+        <v>1891</v>
+      </c>
+    </row>
+    <row r="983" spans="1:2">
       <c r="A983" t="s">
         <v>1012</v>
       </c>
-    </row>
-    <row r="984" spans="1:1">
+      <c r="B983" t="s">
+        <v>1892</v>
+      </c>
+    </row>
+    <row r="984" spans="1:2">
       <c r="A984" t="s">
         <v>1013</v>
       </c>
-    </row>
-    <row r="985" spans="1:1">
+      <c r="B984" t="s">
+        <v>1893</v>
+      </c>
+    </row>
+    <row r="985" spans="1:2">
       <c r="A985" t="s">
         <v>1014</v>
       </c>
-    </row>
-    <row r="986" spans="1:1">
+      <c r="B985" t="s">
+        <v>1420</v>
+      </c>
+    </row>
+    <row r="986" spans="1:2">
       <c r="A986" t="s">
         <v>1015</v>
       </c>
-    </row>
-    <row r="987" spans="1:1">
+      <c r="B986" t="s">
+        <v>1894</v>
+      </c>
+    </row>
+    <row r="987" spans="1:2">
       <c r="A987" t="s">
         <v>1016</v>
       </c>
-    </row>
-    <row r="988" spans="1:1">
+      <c r="B987" t="s">
+        <v>1895</v>
+      </c>
+    </row>
+    <row r="988" spans="1:2">
       <c r="A988" t="s">
         <v>1017</v>
       </c>
-    </row>
-    <row r="989" spans="1:1">
+      <c r="B988" t="s">
+        <v>1896</v>
+      </c>
+    </row>
+    <row r="989" spans="1:2">
       <c r="A989" t="s">
         <v>1018</v>
       </c>
-    </row>
-    <row r="990" spans="1:1">
+      <c r="B989" t="s">
+        <v>1897</v>
+      </c>
+    </row>
+    <row r="990" spans="1:2">
       <c r="A990" t="s">
         <v>1019</v>
       </c>
-    </row>
-    <row r="991" spans="1:1">
+      <c r="B990" t="s">
+        <v>1898</v>
+      </c>
+    </row>
+    <row r="991" spans="1:2">
       <c r="A991" t="s">
         <v>1020</v>
       </c>
-    </row>
-    <row r="992" spans="1:1">
+      <c r="B991" t="s">
+        <v>1899</v>
+      </c>
+    </row>
+    <row r="992" spans="1:2">
       <c r="A992" t="s">
         <v>1021</v>
       </c>
-    </row>
-    <row r="993" spans="1:1">
+      <c r="B992" t="s">
+        <v>1900</v>
+      </c>
+    </row>
+    <row r="993" spans="1:2">
       <c r="A993" t="s">
         <v>1022</v>
       </c>
-    </row>
-    <row r="994" spans="1:1">
+      <c r="B993" t="s">
+        <v>1901</v>
+      </c>
+    </row>
+    <row r="994" spans="1:2">
       <c r="A994" t="s">
         <v>1023</v>
       </c>
-    </row>
-    <row r="995" spans="1:1">
+      <c r="B994" t="s">
+        <v>1902</v>
+      </c>
+    </row>
+    <row r="995" spans="1:2">
       <c r="A995" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="996" spans="1:1">
+      <c r="B995" t="s">
+        <v>1903</v>
+      </c>
+    </row>
+    <row r="996" spans="1:2">
       <c r="A996" t="s">
         <v>1025</v>
       </c>
-    </row>
-    <row r="997" spans="1:1">
+      <c r="B996" t="s">
+        <v>1904</v>
+      </c>
+    </row>
+    <row r="997" spans="1:2">
       <c r="A997" t="s">
         <v>1026</v>
       </c>
-    </row>
-    <row r="998" spans="1:1">
+      <c r="B997" t="s">
+        <v>1905</v>
+      </c>
+    </row>
+    <row r="998" spans="1:2">
       <c r="A998" t="s">
         <v>1027</v>
       </c>
-    </row>
-    <row r="999" spans="1:1">
+      <c r="B998" t="s">
+        <v>1906</v>
+      </c>
+    </row>
+    <row r="999" spans="1:2">
       <c r="A999" t="s">
         <v>1028</v>
       </c>
-    </row>
-    <row r="1000" spans="1:1">
+      <c r="B999" t="s">
+        <v>1907</v>
+      </c>
+    </row>
+    <row r="1000" spans="1:2">
       <c r="A1000" t="s">
         <v>1029</v>
       </c>
-    </row>
-    <row r="1001" spans="1:1">
+      <c r="B1000" t="s">
+        <v>1908</v>
+      </c>
+    </row>
+    <row r="1001" spans="1:2">
       <c r="A1001" t="s">
         <v>1030</v>
       </c>
-    </row>
-    <row r="1002" spans="1:1">
+      <c r="B1001" t="s">
+        <v>1909</v>
+      </c>
+    </row>
+    <row r="1002" spans="1:2">
       <c r="A1002" t="s">
         <v>1031</v>
       </c>
-    </row>
-    <row r="1003" spans="1:1">
+      <c r="B1002" t="s">
+        <v>1910</v>
+      </c>
+    </row>
+    <row r="1003" spans="1:2">
       <c r="A1003" t="s">
         <v>1032</v>
       </c>
-    </row>
-    <row r="1004" spans="1:1">
+      <c r="B1003" t="s">
+        <v>1911</v>
+      </c>
+    </row>
+    <row r="1004" spans="1:2">
       <c r="A1004" t="s">
         <v>1033</v>
       </c>
-    </row>
-    <row r="1005" spans="1:1">
+      <c r="B1004" t="s">
+        <v>1912</v>
+      </c>
+    </row>
+    <row r="1005" spans="1:2">
       <c r="A1005" t="s">
         <v>1034</v>
       </c>
-    </row>
-    <row r="1006" spans="1:1">
+      <c r="B1005" t="s">
+        <v>1913</v>
+      </c>
+    </row>
+    <row r="1006" spans="1:2">
       <c r="A1006" t="s">
         <v>1035</v>
       </c>
-    </row>
-    <row r="1007" spans="1:1">
+      <c r="B1006" t="s">
+        <v>1914</v>
+      </c>
+    </row>
+    <row r="1007" spans="1:2">
       <c r="A1007" t="s">
         <v>1036</v>
       </c>
-    </row>
-    <row r="1008" spans="1:1">
+      <c r="B1007" t="s">
+        <v>1915</v>
+      </c>
+    </row>
+    <row r="1008" spans="1:2">
       <c r="A1008" t="s">
         <v>1037</v>
       </c>
-    </row>
-    <row r="1009" spans="1:1">
+      <c r="B1008" t="s">
+        <v>1916</v>
+      </c>
+    </row>
+    <row r="1009" spans="1:2">
       <c r="A1009" t="s">
         <v>1038</v>
       </c>
-    </row>
-    <row r="1010" spans="1:1">
+      <c r="B1009" t="s">
+        <v>1917</v>
+      </c>
+    </row>
+    <row r="1010" spans="1:2">
       <c r="A1010" t="s">
         <v>1039</v>
       </c>
-    </row>
-    <row r="1011" spans="1:1">
+      <c r="B1010" t="s">
+        <v>1918</v>
+      </c>
+    </row>
+    <row r="1011" spans="1:2">
       <c r="A1011" t="s">
         <v>1040</v>
       </c>
-    </row>
-    <row r="1012" spans="1:1">
+      <c r="B1011" t="s">
+        <v>1919</v>
+      </c>
+    </row>
+    <row r="1012" spans="1:2">
       <c r="A1012" t="s">
         <v>1041</v>
       </c>
-    </row>
-    <row r="1013" spans="1:1">
+      <c r="B1012" t="s">
+        <v>1920</v>
+      </c>
+    </row>
+    <row r="1013" spans="1:2">
       <c r="A1013" t="s">
         <v>1042</v>
       </c>
-    </row>
-    <row r="1014" spans="1:1">
+      <c r="B1013" t="s">
+        <v>1921</v>
+      </c>
+    </row>
+    <row r="1014" spans="1:2">
       <c r="A1014" t="s">
         <v>1043</v>
       </c>
-    </row>
-    <row r="1015" spans="1:1">
+      <c r="B1014" t="s">
+        <v>1922</v>
+      </c>
+    </row>
+    <row r="1015" spans="1:2">
       <c r="A1015" t="s">
         <v>1044</v>
       </c>
-    </row>
-    <row r="1016" spans="1:1">
+      <c r="B1015" t="s">
+        <v>1923</v>
+      </c>
+    </row>
+    <row r="1016" spans="1:2">
       <c r="A1016" t="s">
         <v>1045</v>
       </c>
-    </row>
-    <row r="1017" spans="1:1">
+      <c r="B1016" t="s">
+        <v>1924</v>
+      </c>
+    </row>
+    <row r="1017" spans="1:2">
       <c r="A1017" t="s">
         <v>1046</v>
       </c>
-    </row>
-    <row r="1018" spans="1:1">
+      <c r="B1017" t="s">
+        <v>1946</v>
+      </c>
+    </row>
+    <row r="1018" spans="1:2">
       <c r="A1018" t="s">
         <v>1047</v>
       </c>
-    </row>
-    <row r="1019" spans="1:1">
+      <c r="B1018" t="s">
+        <v>1925</v>
+      </c>
+    </row>
+    <row r="1019" spans="1:2">
       <c r="A1019" t="s">
         <v>1048</v>
       </c>
-    </row>
-    <row r="1020" spans="1:1">
+      <c r="B1019" t="s">
+        <v>1926</v>
+      </c>
+    </row>
+    <row r="1020" spans="1:2">
       <c r="A1020" t="s">
         <v>1049</v>
       </c>
-    </row>
-    <row r="1021" spans="1:1">
+      <c r="B1020" t="s">
+        <v>1927</v>
+      </c>
+    </row>
+    <row r="1021" spans="1:2">
       <c r="A1021" t="s">
         <v>1050</v>
       </c>
-    </row>
-    <row r="1022" spans="1:1">
+      <c r="B1021" t="s">
+        <v>1928</v>
+      </c>
+    </row>
+    <row r="1022" spans="1:2">
       <c r="A1022" t="s">
         <v>1051</v>
       </c>
-    </row>
-    <row r="1023" spans="1:1">
+      <c r="B1022" t="s">
+        <v>1929</v>
+      </c>
+    </row>
+    <row r="1023" spans="1:2">
       <c r="A1023" t="s">
         <v>1052</v>
       </c>
-    </row>
-    <row r="1024" spans="1:1">
+      <c r="B1023" t="s">
+        <v>1930</v>
+      </c>
+    </row>
+    <row r="1024" spans="1:2">
       <c r="A1024" t="s">
         <v>1053</v>
       </c>
-    </row>
-    <row r="1025" spans="1:1">
+      <c r="B1024" t="s">
+        <v>1931</v>
+      </c>
+    </row>
+    <row r="1025" spans="1:2">
       <c r="A1025" t="s">
         <v>1054</v>
       </c>
-    </row>
-    <row r="1026" spans="1:1">
+      <c r="B1025" t="s">
+        <v>1932</v>
+      </c>
+    </row>
+    <row r="1026" spans="1:2">
       <c r="A1026" t="s">
         <v>1055</v>
       </c>
-    </row>
-    <row r="1027" spans="1:1">
+      <c r="B1026" t="s">
+        <v>1933</v>
+      </c>
+    </row>
+    <row r="1027" spans="1:2">
       <c r="A1027" t="s">
         <v>1056</v>
       </c>
-    </row>
-    <row r="1028" spans="1:1">
+      <c r="B1027" t="s">
+        <v>1934</v>
+      </c>
+    </row>
+    <row r="1028" spans="1:2">
       <c r="A1028" t="s">
         <v>1057</v>
       </c>
-    </row>
-    <row r="1029" spans="1:1">
+      <c r="B1028" t="s">
+        <v>1935</v>
+      </c>
+    </row>
+    <row r="1029" spans="1:2">
       <c r="A1029" t="s">
         <v>1058</v>
       </c>
-    </row>
-    <row r="1030" spans="1:1">
+      <c r="B1029" t="s">
+        <v>1936</v>
+      </c>
+    </row>
+    <row r="1030" spans="1:2">
       <c r="A1030" t="s">
         <v>1059</v>
       </c>
-    </row>
-    <row r="1031" spans="1:1">
+      <c r="B1030" t="s">
+        <v>1937</v>
+      </c>
+    </row>
+    <row r="1031" spans="1:2">
       <c r="A1031" t="s">
         <v>1060</v>
       </c>
-    </row>
-    <row r="1032" spans="1:1">
+      <c r="B1031" t="s">
+        <v>1938</v>
+      </c>
+    </row>
+    <row r="1032" spans="1:2">
       <c r="A1032" t="s">
         <v>1061</v>
       </c>
-    </row>
-    <row r="1033" spans="1:1">
+      <c r="B1032" t="s">
+        <v>1939</v>
+      </c>
+    </row>
+    <row r="1033" spans="1:2">
       <c r="A1033" t="s">
         <v>1062</v>
       </c>
-    </row>
-    <row r="1034" spans="1:1">
+      <c r="B1033" t="s">
+        <v>1940</v>
+      </c>
+    </row>
+    <row r="1034" spans="1:2">
       <c r="A1034" t="s">
         <v>1063</v>
       </c>
-    </row>
-    <row r="1035" spans="1:1">
+      <c r="B1034" t="s">
+        <v>1941</v>
+      </c>
+    </row>
+    <row r="1035" spans="1:2">
       <c r="A1035" t="s">
         <v>1064</v>
       </c>
-    </row>
-    <row r="1036" spans="1:1">
+      <c r="B1035" t="s">
+        <v>1942</v>
+      </c>
+    </row>
+    <row r="1036" spans="1:2">
       <c r="A1036" t="s">
         <v>1065</v>
       </c>
-    </row>
-    <row r="1037" spans="1:1">
+      <c r="B1036" t="s">
+        <v>1943</v>
+      </c>
+    </row>
+    <row r="1037" spans="1:2">
       <c r="A1037" t="s">
         <v>1066</v>
       </c>
-    </row>
-    <row r="1038" spans="1:1">
+      <c r="B1037" t="s">
+        <v>1944</v>
+      </c>
+    </row>
+    <row r="1038" spans="1:2">
       <c r="A1038" t="s">
         <v>1067</v>
+      </c>
+      <c r="B1038" t="s">
+        <v>1945</v>
       </c>
     </row>
   </sheetData>

</xml_diff>